<commit_message>
Added time costs for time spent in terminals/harbors
</commit_message>
<xml_diff>
--- a/Data/time_value.xlsx
+++ b/Data/time_value.xlsx
@@ -1,44 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\GitHub\STraM_ntnu_development\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steffejb\OneDrive - NTNU\Work\GitHub\STraM_ntnu_development\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A33F67B-2603-4848-ABD2-EC19F4BA2C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1A33F67B-2603-4848-ABD2-EC19F4BA2C7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{F48A6D00-CF36-4B95-9773-7B3C0E6CB1A2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{611E9C45-D20D-4BC3-B181-B2FEA09DA5CC}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16770" activeTab="3" xr2:uid="{611E9C45-D20D-4BC3-B181-B2FEA09DA5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Time value" sheetId="1" r:id="rId1"/>
     <sheet name="Output" sheetId="2" r:id="rId2"/>
     <sheet name="Speeds" sheetId="3" r:id="rId3"/>
+    <sheet name="TimeInTerminals" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="113">
   <si>
     <t>Jordbruksvarer</t>
   </si>
@@ -374,6 +364,9 @@
   </si>
   <si>
     <t>Sea</t>
+  </si>
+  <si>
+    <t>Time (hours)</t>
   </si>
 </sst>
 </file>
@@ -589,14 +582,14 @@
     <xf numFmtId="2" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -727,10 +720,217 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8549456" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03A893B4-0D03-4D47-B515-F8C7769AE5D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2600325" y="95250"/>
+          <a:ext cx="8549456" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This table provides the average time spent in terminals (harbours/railway terminals), when passing through nodes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> along </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>a path. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>For example, a ship going from Oslo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> to Trondheim might stop in Kristiansand, Stavanger, Bergen, Førde, Ålesund to unload some cargo/containers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>NOTE, when it is an origin or destination node, then the time will be longer.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2407903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD406DC0-3C63-4DBB-AB15-6D6F7DDF1DA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2619375" y="828675"/>
+          <a:ext cx="2407903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Do this for each product class</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> as well?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2471382" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A27C4647-681A-4979-8228-36A369C81554}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="1247775"/>
+          <a:ext cx="2471382" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>THESE NUMBERS NEED TO BE VERIFIED</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3176CB3B-13D2-4839-ABB7-BE835BCA482A}" name="Table1" displayName="Table1" ref="A6:G45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G45" xr:uid="{2177D1D8-2C82-49FC-B7A3-6E60DA922CC3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G45">
+  <sortState ref="A7:G45">
     <sortCondition ref="A6:A45"/>
   </sortState>
   <tableColumns count="7">
@@ -1047,55 +1247,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1D50F6-B75A-4AA5-9462-35F9B49101F5}">
   <dimension ref="A1:AJ146"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC80" sqref="AC80"/>
+    <sheetView topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="5"/>
+    <col min="17" max="17" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" style="5"/>
     <col min="21" max="21" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.88671875" style="5"/>
+    <col min="22" max="22" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="36.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" style="5"/>
     <col min="26" max="26" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="8.88671875" style="5"/>
+    <col min="27" max="27" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="36.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="8.85546875" style="5"/>
     <col min="33" max="33" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="8.88671875" style="5"/>
+    <col min="34" max="34" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="36.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>98</v>
       </c>
@@ -1103,11 +1303,11 @@
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>100</v>
       </c>
@@ -1115,7 +1315,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>102</v>
       </c>
@@ -1141,7 +1341,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
@@ -1166,7 +1366,7 @@
       </c>
       <c r="T7" s="6"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>9</v>
       </c>
@@ -1190,7 +1390,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>30</v>
       </c>
@@ -1214,7 +1414,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>31</v>
       </c>
@@ -1238,7 +1438,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>29</v>
       </c>
@@ -1262,7 +1462,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>22</v>
       </c>
@@ -1286,7 +1486,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>6</v>
       </c>
@@ -1310,7 +1510,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>7</v>
       </c>
@@ -1334,7 +1534,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
@@ -1358,7 +1558,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1582,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +1606,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>24</v>
       </c>
@@ -1430,7 +1630,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>33</v>
       </c>
@@ -1454,7 +1654,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>4</v>
       </c>
@@ -1478,7 +1678,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>32</v>
       </c>
@@ -1502,7 +1702,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -1526,7 +1726,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>2</v>
       </c>
@@ -1550,7 +1750,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>10</v>
       </c>
@@ -1574,7 +1774,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1798,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1822,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>36</v>
       </c>
@@ -1646,7 +1846,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>1</v>
       </c>
@@ -1670,7 +1870,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>20</v>
       </c>
@@ -1694,7 +1894,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>5</v>
       </c>
@@ -1718,7 +1918,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>12</v>
       </c>
@@ -1742,7 +1942,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>19</v>
       </c>
@@ -1766,7 +1966,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>27</v>
       </c>
@@ -1790,7 +1990,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>8</v>
       </c>
@@ -1814,7 +2014,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>18</v>
       </c>
@@ -1838,7 +2038,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>26</v>
       </c>
@@ -1862,7 +2062,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>14</v>
       </c>
@@ -1886,7 +2086,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>28</v>
       </c>
@@ -1910,7 +2110,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>23</v>
       </c>
@@ -1934,7 +2134,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>37</v>
       </c>
@@ -1958,7 +2158,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>34</v>
       </c>
@@ -1982,7 +2182,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>15</v>
       </c>
@@ -2006,7 +2206,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>77</v>
       </c>
@@ -2030,7 +2230,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>16</v>
       </c>
@@ -2054,7 +2254,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>35</v>
       </c>
@@ -2078,7 +2278,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>99</v>
       </c>
@@ -2086,8 +2286,8 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>82</v>
       </c>
@@ -2131,7 +2331,7 @@
       <c r="AI49" s="13"/>
       <c r="AJ49" s="14"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
         <v>92</v>
       </c>
@@ -2217,7 +2417,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <f>IF($F7=A$49,$D7,0)</f>
         <v>0</v>
@@ -2331,7 +2531,7 @@
         <v>0.11190597567079941</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <f t="shared" ref="A52:A89" si="19">IF($F8=A$49,$D8,0)</f>
         <v>0</v>
@@ -2445,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
         <f t="shared" si="19"/>
         <v>0.16000000000000003</v>
@@ -2559,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -2673,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -2787,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -2901,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -3015,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <f t="shared" si="19"/>
         <v>0.16000000000000003</v>
@@ -3129,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -3243,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -3357,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <f t="shared" si="19"/>
         <v>4.0000000000000008E-2</v>
@@ -3471,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -3585,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -3699,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -3813,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <f t="shared" si="19"/>
         <v>0.18000000000000002</v>
@@ -3927,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -4041,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -4155,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <f t="shared" si="19"/>
         <v>0.47000000000000003</v>
@@ -4269,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -4383,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -4497,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <f t="shared" si="19"/>
         <v>0.16000000000000003</v>
@@ -4611,7 +4811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -4725,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -4839,7 +5039,7 @@
         <v>0.84052470602147789</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -4953,7 +5153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -5067,7 +5267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <f t="shared" si="19"/>
         <v>0.16000000000000003</v>
@@ -5181,7 +5381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -5295,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -5409,7 +5609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -5523,7 +5723,7 @@
         <v>1.268145582086044E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -5637,7 +5837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <f t="shared" si="19"/>
         <v>0.48</v>
@@ -5751,7 +5951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -5865,7 +6065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <f t="shared" si="19"/>
         <v>0.16000000000000003</v>
@@ -5979,7 +6179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <f t="shared" si="19"/>
         <v>0.11000000000000001</v>
@@ -6093,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -6207,7 +6407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -6321,7 +6521,7 @@
         <v>1.4736022189147125E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -6435,7 +6635,7 @@
         <v>0.26246655958838327</v>
       </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -6549,7 +6749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -6663,7 +6863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="20" t="s">
         <v>90</v>
       </c>
@@ -6749,12 +6949,12 @@
         <v>1.2423147192906683</v>
       </c>
     </row>
-    <row r="94" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="96" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>74</v>
       </c>
@@ -6762,11 +6962,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I7:K45">
+  <sortState ref="I7:K45">
     <sortCondition ref="I7"/>
   </sortState>
   <mergeCells count="1">
@@ -6788,14 +6988,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>81</v>
       </c>
@@ -6803,7 +7003,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>82</v>
       </c>
@@ -6812,7 +7012,7 @@
         <v>0.13913079978113402</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>84</v>
       </c>
@@ -6821,7 +7021,7 @@
         <v>0.70305272277950881</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>83</v>
       </c>
@@ -6830,7 +7030,7 @@
         <v>9.4716775584260517</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>87</v>
       </c>
@@ -6839,7 +7039,7 @@
         <v>0.50237992716575219</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
@@ -6848,7 +7048,7 @@
         <v>3.0789428630831184</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>85</v>
       </c>
@@ -6857,7 +7057,7 @@
         <v>0.1905058375607222</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>89</v>
       </c>
@@ -6876,24 +7076,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B378C64-8E5B-4630-B6EF-856258632C3E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -6901,7 +7101,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -6909,7 +7109,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -6920,4 +7120,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5EFAB1-6D55-48BF-8108-F84E365EBC38}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated cost calculator connection
</commit_message>
<xml_diff>
--- a/Data/time_value.xlsx
+++ b/Data/time_value.xlsx
@@ -1,34 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steffejb\OneDrive - NTNU\Work\GitHub\STraM_ntnu_development\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1A33F67B-2603-4848-ABD2-EC19F4BA2C7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{F48A6D00-CF36-4B95-9773-7B3C0E6CB1A2}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1A33F67B-2603-4848-ABD2-EC19F4BA2C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC0CF645-718D-44DE-BA5E-D52907F9249A}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16770" activeTab="3" xr2:uid="{611E9C45-D20D-4BC3-B181-B2FEA09DA5CC}"/>
+    <workbookView xWindow="15090" yWindow="690" windowWidth="28800" windowHeight="22170" activeTab="2" xr2:uid="{611E9C45-D20D-4BC3-B181-B2FEA09DA5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Time value" sheetId="1" r:id="rId1"/>
     <sheet name="Output" sheetId="2" r:id="rId2"/>
     <sheet name="Speeds" sheetId="3" r:id="rId3"/>
-    <sheet name="TimeInTerminals" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="112">
   <si>
     <t>Jordbruksvarer</t>
   </si>
@@ -364,9 +374,6 @@
   </si>
   <si>
     <t>Sea</t>
-  </si>
-  <si>
-    <t>Time (hours)</t>
   </si>
 </sst>
 </file>
@@ -720,217 +727,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="8549456" cy="609013"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03A893B4-0D03-4D47-B515-F8C7769AE5D9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2600325" y="95250"/>
-          <a:ext cx="8549456" cy="609013"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>This table provides the average time spent in terminals (harbours/railway terminals), when passing through nodes</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> along </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>a path. </a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1100"/>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>For example, a ship going from Oslo</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> to Trondheim might stop in Kristiansand, Stavanger, Bergen, Førde, Ålesund to unload some cargo/containers</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>NOTE, when it is an origin or destination node, then the time will be longer.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2407903" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD406DC0-3C63-4DBB-AB15-6D6F7DDF1DA8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2619375" y="828675"/>
-          <a:ext cx="2407903" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Do this for each product class</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> as well?</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2471382" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A27C4647-681A-4979-8228-36A369C81554}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2628900" y="1247775"/>
-          <a:ext cx="2471382" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>THESE NUMBERS NEED TO BE VERIFIED</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3176CB3B-13D2-4839-ABB7-BE835BCA482A}" name="Table1" displayName="Table1" ref="A6:G45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G45" xr:uid="{2177D1D8-2C82-49FC-B7A3-6E60DA922CC3}"/>
-  <sortState ref="A7:G45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G45">
     <sortCondition ref="A6:A45"/>
   </sortState>
   <tableColumns count="7">
@@ -1247,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1D50F6-B75A-4AA5-9462-35F9B49101F5}">
   <dimension ref="A1:AJ146"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
@@ -6966,7 +6766,7 @@
       <c r="A146" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="I7:K45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I7:K45">
     <sortCondition ref="I7"/>
   </sortState>
   <mergeCells count="1">
@@ -7076,7 +6876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B378C64-8E5B-4630-B6EF-856258632C3E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -7120,56 +6920,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5EFAB1-6D55-48BF-8108-F84E365EBC38}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>